<commit_message>
Added a new visualisation of the results.
</commit_message>
<xml_diff>
--- a/multimat-bw.xlsx
+++ b/multimat-bw.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="32">
   <si>
     <t>p100</t>
   </si>
@@ -93,14 +93,52 @@
   </si>
   <si>
     <t>P8 (160)</t>
+  </si>
+  <si>
+    <t>vectorised</t>
+  </si>
+  <si>
+    <t>yes</t>
+  </si>
+  <si>
+    <t>compiler inhibits, simd worsens performance marginally</t>
+  </si>
+  <si>
+    <t>compiler inhibits, simd improves performance ~2x on KNL</t>
+  </si>
+  <si>
+    <t>main inner loops not vectorisable, simd outer loop worsens performance</t>
+  </si>
+  <si>
+    <t xml:space="preserve">an inner loop needed simd reduction,  performance </t>
+  </si>
+  <si>
+    <t>inner loop appears unvectorisable, simd outer loop worsens performance</t>
+  </si>
+  <si>
+    <t>inner loop un-vectorisable in current form, simd outer loop worsens performance</t>
+  </si>
+  <si>
+    <t>auto-vectorised</t>
+  </si>
+  <si>
+    <t>vectorising main inner loop requires two simd reductions, marginally worsens performance</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -130,6 +168,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="14"/>
+      <color rgb="FF000000"/>
+      <name val="Helvetica"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -148,23 +192,97 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="5">
+  <cellStyleXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="5">
+  <cellStyles count="41">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="36" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="38" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="40" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="35" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="37" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="39" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -440,48 +558,50 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H43"/>
+  <dimension ref="A1:I54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="B27" sqref="B27"/>
+    <sheetView tabSelected="1" topLeftCell="B53" workbookViewId="0">
+      <selection activeCell="C54" sqref="B47:C54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="15.33203125" customWidth="1"/>
+    <col min="2" max="2" width="19.5" customWidth="1"/>
+    <col min="3" max="3" width="53.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" t="s">
+      <c r="F1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>1</v>
       </c>
       <c r="B2">
         <v>447</v>
       </c>
-      <c r="C2" s="1">
+      <c r="F2" s="1">
         <v>447</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>2</v>
       </c>
       <c r="B3">
         <v>515</v>
       </c>
-      <c r="C3" s="1">
+      <c r="F3" s="1">
         <v>515</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -489,7 +609,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -497,7 +617,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -505,7 +625,7 @@
         <v>418</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -513,7 +633,7 @@
         <v>407</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>8</v>
       </c>
@@ -521,7 +641,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>7</v>
       </c>
@@ -529,24 +649,27 @@
         <v>5</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B16" t="s">
         <v>11</v>
       </c>
       <c r="C16" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D16" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="E16" t="s">
         <v>19</v>
       </c>
       <c r="F16" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="H16" t="s">
         <v>20</v>
+      </c>
+      <c r="I16" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.2">
@@ -557,16 +680,16 @@
         <v>268.39999999999998</v>
       </c>
       <c r="C17">
-        <v>0.54</v>
+        <v>2.23</v>
       </c>
       <c r="D17">
-        <v>1.92</v>
+        <v>1.06</v>
       </c>
       <c r="E17">
-        <v>0.82</v>
+        <v>0.8</v>
       </c>
       <c r="F17">
-        <v>1.17</v>
+        <v>0.49</v>
       </c>
       <c r="H17">
         <v>0.8</v>
@@ -580,16 +703,16 @@
         <v>536.9</v>
       </c>
       <c r="C18">
-        <v>1.04</v>
+        <v>5.24</v>
       </c>
       <c r="D18">
-        <v>5.12</v>
+        <v>2.2599999999999998</v>
       </c>
       <c r="E18">
-        <v>2.17</v>
+        <v>1.87</v>
       </c>
       <c r="F18">
-        <v>2.35</v>
+        <v>1</v>
       </c>
       <c r="H18">
         <v>2.19</v>
@@ -603,16 +726,16 @@
         <v>234.8</v>
       </c>
       <c r="C19">
-        <v>1.1299999999999999</v>
+        <v>7.77</v>
       </c>
       <c r="D19">
-        <v>7.78</v>
+        <v>3.44</v>
       </c>
       <c r="E19">
-        <v>1.88</v>
+        <v>2.67</v>
       </c>
       <c r="F19">
-        <v>3.38</v>
+        <v>1.44</v>
       </c>
       <c r="H19">
         <v>2.72</v>
@@ -626,16 +749,16 @@
         <v>402.5</v>
       </c>
       <c r="C20">
-        <v>2.4700000000000002</v>
+        <v>8.9700000000000006</v>
       </c>
       <c r="D20">
-        <v>10.68</v>
+        <v>5.16</v>
       </c>
       <c r="E20">
         <v>8.4499999999999993</v>
       </c>
       <c r="F20">
-        <v>5.16</v>
+        <v>2.4300000000000002</v>
       </c>
       <c r="H20">
         <v>9.68</v>
@@ -649,16 +772,16 @@
         <v>2080.4</v>
       </c>
       <c r="C21">
+        <v>19.82</v>
+      </c>
+      <c r="D21">
+        <v>9.74</v>
+      </c>
+      <c r="E21">
+        <v>15.83</v>
+      </c>
+      <c r="F21">
         <v>20.77</v>
-      </c>
-      <c r="D21">
-        <v>19.82</v>
-      </c>
-      <c r="E21">
-        <v>15.93</v>
-      </c>
-      <c r="F21">
-        <v>12.6</v>
       </c>
       <c r="H21">
         <v>18.05</v>
@@ -672,16 +795,16 @@
         <v>536.9</v>
       </c>
       <c r="C22">
-        <v>51.89</v>
+        <v>7.28</v>
       </c>
       <c r="D22">
-        <v>7.28</v>
+        <v>4.13</v>
       </c>
       <c r="E22">
-        <v>10.050000000000001</v>
+        <v>4.18</v>
       </c>
       <c r="F22">
-        <v>8.2200000000000006</v>
+        <v>6.78</v>
       </c>
       <c r="H22">
         <v>9.4700000000000006</v>
@@ -695,16 +818,16 @@
         <v>37940.400000000001</v>
       </c>
       <c r="C23">
-        <v>34.64</v>
+        <v>170.77</v>
       </c>
       <c r="D23">
-        <v>170.77</v>
+        <v>81.819999999999993</v>
       </c>
       <c r="E23">
         <v>80.5</v>
       </c>
       <c r="F23">
-        <v>81.819999999999993</v>
+        <v>34.64</v>
       </c>
       <c r="H23">
         <v>91.9</v>
@@ -718,16 +841,16 @@
         <v>45791</v>
       </c>
       <c r="C24">
-        <v>1154.6500000000001</v>
+        <v>389.23</v>
       </c>
       <c r="D24">
-        <v>389.23</v>
+        <v>171.93</v>
       </c>
       <c r="E24">
         <v>175.04</v>
       </c>
       <c r="F24">
-        <v>171.93</v>
+        <v>1154.6500000000001</v>
       </c>
       <c r="H24">
         <v>191.63</v>
@@ -738,16 +861,16 @@
         <v>9</v>
       </c>
       <c r="C25">
-        <v>500</v>
+        <v>130</v>
       </c>
       <c r="D25">
-        <v>130</v>
+        <v>298</v>
       </c>
       <c r="E25">
         <v>450</v>
       </c>
       <c r="F25">
-        <v>298</v>
+        <v>550</v>
       </c>
       <c r="H25">
         <v>450</v>
@@ -756,19 +879,19 @@
     <row r="27" spans="1:8" x14ac:dyDescent="0.2">
       <c r="C27">
         <f>B17/(C17/1000)/1024</f>
-        <v>485.38773148148141</v>
+        <v>117.53783632286995</v>
       </c>
       <c r="D27">
-        <f>B17/(D17/1000)/1024</f>
-        <v>136.51529947916666</v>
+        <f>$B17/(D17/1000)/1024</f>
+        <v>247.27299528301884</v>
       </c>
       <c r="E27">
         <f>$B17/(E17/1000)/1024</f>
-        <v>319.64557926829264</v>
+        <v>327.63671874999994</v>
       </c>
       <c r="F27">
-        <f>$B17/(F17/1000)/1024</f>
-        <v>224.02510683760681</v>
+        <f>B17/(F17/1000)/1024</f>
+        <v>534.9170918367347</v>
       </c>
       <c r="H27">
         <f>$B17/(H17/1000)/1024</f>
@@ -778,19 +901,19 @@
     <row r="28" spans="1:8" x14ac:dyDescent="0.2">
       <c r="C28">
         <f>B18/(C18/1000)/1024</f>
-        <v>504.15039062499994</v>
+        <v>100.06038287213741</v>
       </c>
       <c r="D28">
-        <f>B18/(D18/1000)/1024</f>
-        <v>102.40554809570311</v>
+        <f>$B18/(D18/1000)/1024</f>
+        <v>231.99840984513276</v>
       </c>
       <c r="E28">
         <f>B18/(E18/1000)/1024</f>
-        <v>241.62046370967741</v>
+        <v>280.38310494652404</v>
       </c>
       <c r="F28">
-        <f>$B18/(F18/1000)/1024</f>
-        <v>223.11336436170211</v>
+        <f>B18/(F18/1000)/1024</f>
+        <v>524.31640625</v>
       </c>
       <c r="H28">
         <f>$B18/(H18/1000)/1024</f>
@@ -800,19 +923,19 @@
     <row r="29" spans="1:8" x14ac:dyDescent="0.2">
       <c r="C29">
         <f>B19/(C19/1000)/1024</f>
-        <v>202.91758849557525</v>
+        <v>29.510537323037326</v>
       </c>
       <c r="D29">
-        <f>B19/(D19/1000)/1024</f>
-        <v>29.472606041131105</v>
+        <f>$B19/(D19/1000)/1024</f>
+        <v>66.656068313953497</v>
       </c>
       <c r="E29">
         <f>B19/(E19/1000)/1024</f>
-        <v>121.96642287234043</v>
+        <v>85.87897940074906</v>
       </c>
       <c r="F29">
-        <f>$B19/(F19/1000)/1024</f>
-        <v>67.839312130177518</v>
+        <f>B19/(F19/1000)/1024</f>
+        <v>159.23394097222226</v>
       </c>
       <c r="H29">
         <f>$B19/(H19/1000)/1024</f>
@@ -822,19 +945,19 @@
     <row r="30" spans="1:8" x14ac:dyDescent="0.2">
       <c r="C30">
         <f>B20/(C20/1000)/1024</f>
-        <v>159.13619686234816</v>
+        <v>43.820112179487175</v>
       </c>
       <c r="D30">
-        <f>B20/(D20/1000)/1024</f>
-        <v>36.803970622659172</v>
+        <f>$B20/(D20/1000)/1024</f>
+        <v>76.175660125968989</v>
       </c>
       <c r="E30">
         <f>B20/(E20/1000)/1024</f>
         <v>46.516734467455628</v>
       </c>
       <c r="F30">
-        <f>$B20/(F20/1000)/1024</f>
-        <v>76.175660125968989</v>
+        <f>B20/(F20/1000)/1024</f>
+        <v>161.7557227366255</v>
       </c>
       <c r="H30">
         <f>$B20/(H20/1000)/1024</f>
@@ -844,19 +967,19 @@
     <row r="31" spans="1:8" x14ac:dyDescent="0.2">
       <c r="C31">
         <f>B23/(C23/1000)/1024</f>
-        <v>1069.6065783775982</v>
+        <v>216.96534446916905</v>
       </c>
       <c r="D31">
-        <f>B23/(D23/1000)/1024</f>
-        <v>216.96534446916905</v>
+        <f>$B23/(D23/1000)/1024</f>
+        <v>452.83759319237356</v>
       </c>
       <c r="E31">
         <f>B23/(E23/1000)/1024</f>
         <v>460.26300465838511</v>
       </c>
       <c r="F31">
-        <f>$B23/(F23/1000)/1024</f>
-        <v>452.83759319237356</v>
+        <f>B23/(F23/1000)/1024</f>
+        <v>1069.6065783775982</v>
       </c>
       <c r="H31">
         <f>$B23/(H23/1000)/1024</f>
@@ -866,230 +989,248 @@
     <row r="32" spans="1:8" x14ac:dyDescent="0.2">
       <c r="C32">
         <f>B21/(C21/1000)/1024</f>
-        <v>97.81611097737121</v>
+        <v>102.50457240161452</v>
       </c>
       <c r="D32">
-        <f>B21/(D21/1000)/1024</f>
-        <v>102.50457240161452</v>
+        <f>$B21/(D21/1000)/1024</f>
+        <v>208.58733316221765</v>
       </c>
       <c r="E32">
         <f>B21/(E21/1000)/1024</f>
-        <v>127.5355069052103</v>
+        <v>128.34116392924827</v>
       </c>
       <c r="F32">
-        <f>$B21/(F21/1000)/1024</f>
-        <v>161.24131944444446</v>
+        <f>B21/(F21/1000)/1024</f>
+        <v>97.81611097737121</v>
       </c>
       <c r="H32">
         <f>$B21/(H21/1000)/1024</f>
         <v>112.55626731301939</v>
       </c>
     </row>
-    <row r="33" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="33" spans="2:9" x14ac:dyDescent="0.2">
       <c r="C33">
         <f>B22/(C22/1000)/1024</f>
-        <v>10.104382467720177</v>
+        <v>72.021484375</v>
       </c>
       <c r="D33">
-        <f>B22/(D22/1000)/1024</f>
-        <v>72.021484375</v>
+        <f>$B22/(D22/1000)/1024</f>
+        <v>126.953125</v>
       </c>
       <c r="E33">
         <f>B22/(E22/1000)/1024</f>
-        <v>52.17078669154229</v>
+        <v>125.43454694976077</v>
       </c>
       <c r="F33">
-        <f>$B22/(F22/1000)/1024</f>
-        <v>63.785450881995132</v>
+        <f>B22/(F22/1000)/1024</f>
+        <v>77.332803281710909</v>
       </c>
       <c r="H33">
         <f>$B22/(H22/1000)/1024</f>
         <v>55.366040786694818</v>
       </c>
     </row>
-    <row r="34" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="34" spans="2:9" x14ac:dyDescent="0.2">
       <c r="C34">
         <f>B24/(C24/1000)/1024</f>
-        <v>38.728422844584934</v>
+        <v>114.88778726588392</v>
       </c>
       <c r="D34">
-        <f>B24/(D24/1000)/1024</f>
-        <v>114.88778726588392</v>
+        <f>$B24/(D24/1000)/1024</f>
+        <v>260.09290663351362</v>
       </c>
       <c r="E34">
         <f>B24/(E24/1000)/1024</f>
         <v>255.47174038791132</v>
       </c>
       <c r="F34">
-        <f t="shared" ref="F34" si="0">$B24/(F24/1000)/1024</f>
-        <v>260.09290663351362</v>
+        <f>B24/(F24/1000)/1024</f>
+        <v>38.728422844584934</v>
       </c>
       <c r="H34">
         <f>$B24/(H24/1000)/1024</f>
         <v>233.35476406356</v>
       </c>
     </row>
-    <row r="36" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="36" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B36" t="s">
         <v>16</v>
       </c>
       <c r="C36" s="2">
         <f>C27/$C$25</f>
-        <v>0.9707754629629628</v>
+        <v>0.90413720248361495</v>
       </c>
       <c r="D36" s="2">
         <f>D27/$D$25</f>
-        <v>1.0501176883012819</v>
+        <v>0.82977515195643903</v>
       </c>
       <c r="E36" s="2">
         <f>E27/$E$25</f>
-        <v>0.71032350948509471</v>
+        <v>0.7280815972222221</v>
       </c>
       <c r="F36" s="2">
         <f>F27/$F$25</f>
-        <v>0.75176210348190209</v>
+        <v>0.97257653061224492</v>
       </c>
       <c r="H36" s="2">
         <f>H27/$H$25</f>
         <v>0.7280815972222221</v>
       </c>
-    </row>
-    <row r="37" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="I36" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="37" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B37" t="s">
         <v>2</v>
       </c>
       <c r="C37" s="2">
-        <f t="shared" ref="C37:C39" si="1">C28/$C$25</f>
-        <v>1.0083007812499998</v>
+        <f>C28/$C$25</f>
+        <v>0.76969525286259544</v>
       </c>
       <c r="D37" s="2">
-        <f t="shared" ref="D37:D39" si="2">D28/$D$25</f>
-        <v>0.78773498535156239</v>
+        <f>D28/$D$25</f>
+        <v>0.77851815384272738</v>
       </c>
       <c r="E37" s="2">
-        <f t="shared" ref="E37:E39" si="3">E28/$E$25</f>
-        <v>0.53693436379928317</v>
+        <f>E28/$E$25</f>
+        <v>0.62307356654783119</v>
       </c>
       <c r="F37" s="2">
-        <f t="shared" ref="F37:F39" si="4">F28/$F$25</f>
-        <v>0.7487025649721547</v>
+        <f t="shared" ref="F37:F39" si="0">F28/$F$25</f>
+        <v>0.95330255681818177</v>
       </c>
       <c r="H37" s="2">
         <f>H28/$H$25</f>
         <v>0.53203085362760016</v>
       </c>
-    </row>
-    <row r="38" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="I37" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="38" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B38" t="s">
         <v>12</v>
       </c>
       <c r="C38" s="2">
-        <f t="shared" si="1"/>
-        <v>0.40583517699115051</v>
+        <f>C29/$C$25</f>
+        <v>0.22700413325413327</v>
       </c>
       <c r="D38" s="2">
-        <f t="shared" si="2"/>
-        <v>0.22671235416254695</v>
+        <f>D29/$D$25</f>
+        <v>0.22367808159044797</v>
       </c>
       <c r="E38" s="2">
-        <f t="shared" si="3"/>
-        <v>0.27103649527186763</v>
+        <f>E29/$E$25</f>
+        <v>0.19084217644610901</v>
       </c>
       <c r="F38" s="2">
-        <f t="shared" si="4"/>
-        <v>0.22764869842341448</v>
+        <f t="shared" si="0"/>
+        <v>0.28951625631313138</v>
       </c>
       <c r="H38" s="2">
         <f>H29/$H$25</f>
         <v>0.18733404820261437</v>
       </c>
-    </row>
-    <row r="39" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="I38" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="39" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B39" t="s">
         <v>6</v>
       </c>
       <c r="C39" s="2">
-        <f t="shared" si="1"/>
-        <v>0.31827239372469629</v>
+        <f>C30/$C$25</f>
+        <v>0.3370777859960552</v>
       </c>
       <c r="D39" s="2">
-        <f t="shared" si="2"/>
-        <v>0.28310746632814748</v>
+        <f>D30/$D$25</f>
+        <v>0.25562302055694291</v>
       </c>
       <c r="E39" s="2">
-        <f t="shared" si="3"/>
+        <f>E30/$E$25</f>
         <v>0.10337052103879028</v>
       </c>
       <c r="F39" s="2">
-        <f t="shared" si="4"/>
-        <v>0.25562302055694291</v>
+        <f t="shared" si="0"/>
+        <v>0.29410131406659185</v>
       </c>
       <c r="H39" s="2">
         <f>H30/$H$25</f>
         <v>9.0235630452249777E-2</v>
       </c>
-    </row>
-    <row r="40" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="I39" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="40" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B40" t="s">
         <v>14</v>
       </c>
       <c r="C40" s="2">
         <f>C32/$C$25</f>
-        <v>0.19563222195474242</v>
+        <v>0.78849671078165018</v>
       </c>
       <c r="D40" s="2">
         <f>D32/$D$25</f>
-        <v>0.78849671078165018</v>
+        <v>0.69995749383294514</v>
       </c>
       <c r="E40" s="2">
         <f>E32/$E$25</f>
-        <v>0.28341223756713402</v>
+        <v>0.28520258650944058</v>
       </c>
       <c r="F40" s="2">
         <f>F32/$F$25</f>
-        <v>0.54107825316927671</v>
+        <v>0.17784747450431129</v>
       </c>
       <c r="H40" s="2">
         <f>H32/$H$25</f>
         <v>0.25012503847337642</v>
       </c>
-    </row>
-    <row r="41" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="I40" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="41" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B41" t="s">
         <v>4</v>
       </c>
       <c r="C41" s="2">
         <f>C33/$C$25</f>
-        <v>2.0208764935440354E-2</v>
+        <v>0.55401141826923073</v>
       </c>
       <c r="D41" s="2">
         <f>D33/$D$25</f>
-        <v>0.55401141826923073</v>
+        <v>0.42601719798657717</v>
       </c>
       <c r="E41" s="2">
         <f>E33/$E$25</f>
-        <v>0.11593508153676065</v>
+        <v>0.27874343766613507</v>
       </c>
       <c r="F41" s="2">
         <f>F33/$F$25</f>
-        <v>0.21404513718790313</v>
+        <v>0.14060509687583803</v>
       </c>
       <c r="H41" s="2">
         <f>H33/$H$25</f>
         <v>0.12303564619265515</v>
       </c>
-    </row>
-    <row r="42" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="I41" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="42" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B42" t="s">
         <v>13</v>
       </c>
       <c r="C42" s="2">
         <f>C31/$C$25</f>
-        <v>2.1392131567551966</v>
+        <v>1.6689641882243773</v>
       </c>
       <c r="D42" s="2">
         <f>D31/$D$25</f>
-        <v>1.6689641882243773</v>
+        <v>1.5195892389005825</v>
       </c>
       <c r="E42" s="2">
         <f>E31/$E$25</f>
@@ -1097,24 +1238,27 @@
       </c>
       <c r="F42" s="2">
         <f>F31/$F$25</f>
-        <v>1.5195892389005825</v>
+        <v>1.9447392334138149</v>
       </c>
       <c r="H42" s="2">
         <f>H31/$H$25</f>
         <v>0.89592967899891174</v>
       </c>
-    </row>
-    <row r="43" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="I42" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="43" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B43" t="s">
         <v>15</v>
       </c>
       <c r="C43" s="2">
         <f>C34/$C$25</f>
-        <v>7.745684568916987E-2</v>
+        <v>0.88375220973756863</v>
       </c>
       <c r="D43" s="2">
         <f>D34/$D$25</f>
-        <v>0.88375220973756863</v>
+        <v>0.87279498870306582</v>
       </c>
       <c r="E43" s="2">
         <f>E34/$E$25</f>
@@ -1122,12 +1266,111 @@
       </c>
       <c r="F43" s="2">
         <f>F34/$F$25</f>
-        <v>0.87279498870306582</v>
+        <v>7.0415314262881695E-2</v>
       </c>
       <c r="H43" s="2">
         <f>H34/$H$25</f>
         <v>0.51856614236346665</v>
       </c>
+      <c r="I43" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="47" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B47" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C47" t="s">
+        <v>30</v>
+      </c>
+      <c r="D47" s="2"/>
+      <c r="E47" s="2"/>
+      <c r="F47" s="2"/>
+      <c r="H47" s="2"/>
+    </row>
+    <row r="48" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B48" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C48" t="s">
+        <v>30</v>
+      </c>
+      <c r="D48" s="2"/>
+      <c r="E48" s="2"/>
+      <c r="F48" s="2"/>
+      <c r="H48" s="2"/>
+    </row>
+    <row r="49" spans="2:8" ht="18" x14ac:dyDescent="0.2">
+      <c r="B49" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C49" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="D49" s="2"/>
+      <c r="E49" s="2"/>
+      <c r="F49" s="2"/>
+      <c r="H49" s="2"/>
+    </row>
+    <row r="50" spans="2:8" ht="18" x14ac:dyDescent="0.2">
+      <c r="B50" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C50" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="D50" s="2"/>
+      <c r="E50" s="2"/>
+      <c r="F50" s="2"/>
+      <c r="H50" s="2"/>
+    </row>
+    <row r="51" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B51" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C51" t="s">
+        <v>24</v>
+      </c>
+      <c r="D51" s="2"/>
+      <c r="E51" s="2"/>
+      <c r="F51" s="2"/>
+      <c r="H51" s="2"/>
+    </row>
+    <row r="52" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B52" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C52" t="s">
+        <v>25</v>
+      </c>
+      <c r="D52" s="2"/>
+      <c r="E52" s="2"/>
+      <c r="F52" s="2"/>
+      <c r="H52" s="2"/>
+    </row>
+    <row r="53" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B53" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C53" t="s">
+        <v>26</v>
+      </c>
+      <c r="D53" s="2"/>
+      <c r="E53" s="2"/>
+      <c r="F53" s="2"/>
+      <c r="H53" s="2"/>
+    </row>
+    <row r="54" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B54" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C54" t="s">
+        <v>31</v>
+      </c>
+      <c r="D54" s="2"/>
+      <c r="E54" s="2"/>
+      <c r="F54" s="2"/>
+      <c r="H54" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>